<commit_message>
feuille de temps du 1 septembre
</commit_message>
<xml_diff>
--- a/Document/Feuille de temps.xlsx
+++ b/Document/Feuille de temps.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="9780"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille de temps" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="28-aout" sheetId="1" r:id="rId1"/>
+    <sheet name="1-sept" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>setter l'environnement pour le projet</t>
+  </si>
+  <si>
+    <t>préparer Kanban</t>
+  </si>
+  <si>
+    <t>Plan BD</t>
   </si>
 </sst>
 </file>
@@ -112,7 +118,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="dd/mmm"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
@@ -137,6 +152,20 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E32" totalsRowShown="0">
+  <autoFilter ref="A1:E32"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Nom"/>
+    <tableColumn id="2" name="Date" dataDxfId="5"/>
+    <tableColumn id="3" name="Heure début" dataDxfId="4"/>
+    <tableColumn id="4" name="Heure fin" dataDxfId="3"/>
+    <tableColumn id="5" name="Tâche"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E32" totalsRowShown="0">
   <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Nom"/>
@@ -438,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,96 +699,168 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -775,13 +876,266 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ajout du doc de planification 1 et du login idd Update de la feuille de temps
</commit_message>
<xml_diff>
--- a/Document/Feuille de temps.xlsx
+++ b/Document/Feuille de temps.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="28-aout" sheetId="1" r:id="rId1"/>
     <sheet name="1-sept" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="3-sept" sheetId="3" r:id="rId3"/>
+    <sheet name="4-sept" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +76,15 @@
   </si>
   <si>
     <t>Plan BD</t>
+  </si>
+  <si>
+    <t>makette</t>
+  </si>
+  <si>
+    <t>Content Matrix</t>
+  </si>
+  <si>
+    <t>Planification phase 1</t>
   </si>
 </sst>
 </file>
@@ -118,7 +128,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="dd/mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="dd/mmm"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
@@ -155,6 +183,34 @@
   <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Nom"/>
+    <tableColumn id="2" name="Date" dataDxfId="11"/>
+    <tableColumn id="3" name="Heure début" dataDxfId="10"/>
+    <tableColumn id="4" name="Heure fin" dataDxfId="9"/>
+    <tableColumn id="5" name="Tâche"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E32" totalsRowShown="0">
+  <autoFilter ref="A1:E32"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Nom"/>
+    <tableColumn id="2" name="Date" dataDxfId="8"/>
+    <tableColumn id="3" name="Heure début" dataDxfId="7"/>
+    <tableColumn id="4" name="Heure fin" dataDxfId="6"/>
+    <tableColumn id="5" name="Tâche"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau134" displayName="Tableau134" ref="A1:E32" totalsRowShown="0">
+  <autoFilter ref="A1:E32"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Nom"/>
     <tableColumn id="2" name="Date" dataDxfId="5"/>
     <tableColumn id="3" name="Heure début" dataDxfId="4"/>
     <tableColumn id="4" name="Heure fin" dataDxfId="3"/>
@@ -164,8 +220,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E32" totalsRowShown="0">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau1345" displayName="Tableau1345" ref="A1:E32" totalsRowShown="0">
   <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Nom"/>
@@ -467,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,12 +1197,518 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42250</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42250</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42250</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42250</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42250</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42250</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42251</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42251</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42251</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42251</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42251</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de la base de donné, modification du plan de la bd modification de la feuille de temps ajout du plan pour la phase 1 supression de fichier inutiles
</commit_message>
<xml_diff>
--- a/Document/Feuille de temps.xlsx
+++ b/Document/Feuille de temps.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="28-aout" sheetId="1" r:id="rId1"/>
@@ -1199,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1464,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>42251</v>
@@ -1521,12 +1521,12 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>42251</v>
@@ -1543,36 +1543,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>42251</v>
       </c>
       <c r="C5" s="2">
-        <v>0.35416666666666669</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D5" s="2">
         <v>0.52083333333333337</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>42251</v>
       </c>
       <c r="C6" s="2">
-        <v>0.36458333333333331</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D6" s="2">
         <v>0.52083333333333337</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout du script de création de la bd Modification de la feuille de temps
</commit_message>
<xml_diff>
--- a/Document/Feuille de temps.xlsx
+++ b/Document/Feuille de temps.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="28-aout" sheetId="1" r:id="rId1"/>
     <sheet name="1-sept" sheetId="2" r:id="rId2"/>
     <sheet name="3-sept" sheetId="3" r:id="rId3"/>
     <sheet name="4-sept" sheetId="4" r:id="rId4"/>
+    <sheet name="8-sept" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +86,18 @@
   </si>
   <si>
     <t>Planification phase 1</t>
+  </si>
+  <si>
+    <t>Plan Bd</t>
+  </si>
+  <si>
+    <t>content matrix</t>
+  </si>
+  <si>
+    <t>maquette</t>
+  </si>
+  <si>
+    <t>bd</t>
   </si>
 </sst>
 </file>
@@ -128,7 +141,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="dd/mmm"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
@@ -183,6 +205,20 @@
   <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Nom"/>
+    <tableColumn id="2" name="Date" dataDxfId="14"/>
+    <tableColumn id="3" name="Heure début" dataDxfId="13"/>
+    <tableColumn id="4" name="Heure fin" dataDxfId="12"/>
+    <tableColumn id="5" name="Tâche"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E32" totalsRowShown="0">
+  <autoFilter ref="A1:E32"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Nom"/>
     <tableColumn id="2" name="Date" dataDxfId="11"/>
     <tableColumn id="3" name="Heure début" dataDxfId="10"/>
     <tableColumn id="4" name="Heure fin" dataDxfId="9"/>
@@ -192,8 +228,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E32" totalsRowShown="0">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau134" displayName="Tableau134" ref="A1:E32" totalsRowShown="0">
   <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Nom"/>
@@ -206,8 +242,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau134" displayName="Tableau134" ref="A1:E32" totalsRowShown="0">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau1345" displayName="Tableau1345" ref="A1:E32" totalsRowShown="0">
   <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Nom"/>
@@ -220,8 +256,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau1345" displayName="Tableau1345" ref="A1:E32" totalsRowShown="0">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau13456" displayName="Tableau13456" ref="A1:E32" totalsRowShown="0">
   <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Nom"/>
@@ -1200,7 +1236,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection sqref="A1:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1574,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,7 +1608,272 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42251</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42255</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42255</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42255</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42255</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42255</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update de la feuille de temps et de la maquette
</commit_message>
<xml_diff>
--- a/Document/Feuille de temps.xlsx
+++ b/Document/Feuille de temps.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>bd</t>
+  </si>
+  <si>
+    <t>mise à jour des docs</t>
   </si>
 </sst>
 </file>
@@ -1766,7 +1769,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,9 +1880,21 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42255</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>

</xml_diff>

<commit_message>
modification de la feuille de temps
</commit_message>
<xml_diff>
--- a/Document/Feuille de temps.xlsx
+++ b/Document/Feuille de temps.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>mise à jour des docs</t>
+  </si>
+  <si>
+    <t>idd</t>
   </si>
 </sst>
 </file>
@@ -1769,7 +1772,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,9 +1900,21 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42255</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>

</xml_diff>